<commit_message>
9/17/22 Created System Set Point FIles
</commit_message>
<xml_diff>
--- a/RLRMDB/DataFiles/MaterialData.xlsx
+++ b/RLRMDB/DataFiles/MaterialData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TBeck\WorkDB\RLRMDB\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37A712B-C075-494C-B490-D42486679E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C14A7EB-3D1D-4D46-B2EA-FEC0B365A5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{721B2988-C9D0-4D28-A3CB-1893A34E73F2}"/>
+    <workbookView xWindow="3840" yWindow="1932" windowWidth="18900" windowHeight="10248" xr2:uid="{721B2988-C9D0-4D28-A3CB-1893A34E73F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -313,12 +313,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -635,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CAE0AA-16CC-4652-A654-F145712A7B81}">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +729,7 @@
       <c r="B2" t="s">
         <v>53</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="3">
         <v>58971</v>
       </c>
       <c r="D2" t="s">
@@ -787,7 +788,7 @@
       <c r="B3" t="s">
         <v>54</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="3">
         <v>58423</v>
       </c>
       <c r="D3" t="s">
@@ -846,7 +847,7 @@
       <c r="B4" t="s">
         <v>55</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="3">
         <v>58913</v>
       </c>
       <c r="D4" t="s">
@@ -905,7 +906,7 @@
       <c r="B5" t="s">
         <v>56</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>58245</v>
       </c>
       <c r="D5" t="s">
@@ -964,7 +965,7 @@
       <c r="B6" t="s">
         <v>57</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>58143</v>
       </c>
       <c r="D6" t="s">
@@ -1023,7 +1024,7 @@
       <c r="B7" t="s">
         <v>58</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>58765</v>
       </c>
       <c r="D7" t="s">
@@ -1082,7 +1083,7 @@
       <c r="B8" t="s">
         <v>53</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="3">
         <v>31777</v>
       </c>
       <c r="N8">
@@ -1111,7 +1112,7 @@
       <c r="B9" t="s">
         <v>54</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="3">
         <v>36178</v>
       </c>
       <c r="N9">
@@ -1140,7 +1141,7 @@
       <c r="B10" t="s">
         <v>55</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>32144</v>
       </c>
       <c r="N10">
@@ -1169,7 +1170,7 @@
       <c r="B11" t="s">
         <v>56</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="3">
         <v>32716</v>
       </c>
       <c r="N11">
@@ -1198,7 +1199,7 @@
       <c r="B12" t="s">
         <v>57</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>32409</v>
       </c>
       <c r="N12">
@@ -1227,7 +1228,7 @@
       <c r="B13" t="s">
         <v>58</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="3">
         <v>30173</v>
       </c>
       <c r="N13">
@@ -1256,7 +1257,7 @@
       <c r="B14" t="s">
         <v>53</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="3">
         <v>3282571</v>
       </c>
       <c r="N14">
@@ -1285,7 +1286,7 @@
       <c r="B15" t="s">
         <v>54</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="3">
         <v>3322187</v>
       </c>
       <c r="N15">
@@ -1314,7 +1315,7 @@
       <c r="B16" t="s">
         <v>55</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="3">
         <v>3665760</v>
       </c>
       <c r="N16">
@@ -1343,7 +1344,7 @@
       <c r="B17" t="s">
         <v>56</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="3">
         <v>3081971</v>
       </c>
       <c r="N17">
@@ -1372,7 +1373,7 @@
       <c r="B18" t="s">
         <v>57</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="3">
         <v>3589067</v>
       </c>
       <c r="N18">
@@ -1401,7 +1402,7 @@
       <c r="B19" t="s">
         <v>58</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="3">
         <v>3579790</v>
       </c>
       <c r="N19">
@@ -1430,7 +1431,7 @@
       <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="3">
         <v>3372033</v>
       </c>
       <c r="N20">
@@ -1459,7 +1460,7 @@
       <c r="B21" t="s">
         <v>54</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>3195356</v>
       </c>
       <c r="N21">
@@ -1488,7 +1489,7 @@
       <c r="B22" t="s">
         <v>55</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="3">
         <v>3531374</v>
       </c>
       <c r="N22">
@@ -1517,7 +1518,7 @@
       <c r="B23" t="s">
         <v>56</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="3">
         <v>3948173</v>
       </c>
       <c r="N23">
@@ -1546,7 +1547,7 @@
       <c r="B24" t="s">
         <v>57</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>3473903</v>
       </c>
       <c r="N24">
@@ -1575,7 +1576,7 @@
       <c r="B25" t="s">
         <v>58</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="3">
         <v>3789434</v>
       </c>
       <c r="N25">

</xml_diff>